<commit_message>
mod passroot, add class diagram
</commit_message>
<xml_diff>
--- a/API定義書.xlsx
+++ b/API定義書.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="14805" windowHeight="7995" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="購入履歴一覧表示API" sheetId="1" r:id="rId1"/>
     <sheet name="支払詳細API " sheetId="3" r:id="rId2"/>
     <sheet name="品目一覧取得API" sheetId="4" r:id="rId3"/>
+    <sheet name="クラス図" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="82">
   <si>
     <t>API和名</t>
     <rPh sb="3" eb="5">
@@ -280,10 +281,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>paymentDetail</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>呼出パラメータをもとに購入履歴一覧テーブルに購入履歴を挿入する。</t>
     <rPh sb="0" eb="2">
       <t>ヨビダシ</t>
@@ -340,10 +337,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>POST: api/payment/paymentList/</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>STRING</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -377,10 +370,6 @@
     <rPh sb="8" eb="10">
       <t>エイメイ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>POST: api/payment/paymentDetail/</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -431,18 +420,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>getItemList</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>呼出パラメータ</t>
     <rPh sb="0" eb="2">
       <t>ヨビダシ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>POST: api/payment/getItemList/</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -492,10 +473,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>itemId</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>品目一覧を返却する。</t>
     <rPh sb="0" eb="2">
       <t>ヒンモク</t>
@@ -506,6 +483,97 @@
     <rPh sb="5" eb="7">
       <t>ヘンキャク</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>itemId</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>amount</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>購入履歴一覧表示API</t>
+  </si>
+  <si>
+    <t>itemId</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>POST: api/paymentList/</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>POST: api/paymentDetail/</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>POST: api/getItemList/</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PaymentListRestController</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PaymentListRepositoryService</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PaymentListService</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>支払詳細API</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>paymentDetail</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PaymentDetailRestController</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PaymentDetailService</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>品目一覧取得API</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>getItemList</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>GetItemListRestController</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>GetItemListService</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>GetItemListRepositoryService</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Item</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PaymentInfoDB</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PaymentInfo</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>QueryInfo</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -552,7 +620,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -647,11 +715,62 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -697,6 +816,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -709,6 +850,652 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="直線コネクタ 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2190750" y="866775"/>
+          <a:ext cx="390525" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="直線コネクタ 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3619500" y="866775"/>
+          <a:ext cx="847725" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="直線コネクタ 6"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2752725" y="657225"/>
+          <a:ext cx="666750" cy="19050"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln cap="sq">
+          <a:prstDash val="sysDash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="直線コネクタ 9"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5524500" y="685800"/>
+          <a:ext cx="657225" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="sysDash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="直線コネクタ 11"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5210175" y="1257300"/>
+          <a:ext cx="1095375" cy="971550"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="sysDash"/>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="直線コネクタ 13"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8229600" y="1019175"/>
+          <a:ext cx="704850" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="直線コネクタ 15"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2752725" y="2400300"/>
+          <a:ext cx="676275" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="sysDash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="直線コネクタ 17"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2286000" y="2590800"/>
+          <a:ext cx="419100" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="直線コネクタ 19"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3705225" y="2600325"/>
+          <a:ext cx="381000" cy="142875"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="直線コネクタ 21"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2762250" y="3971925"/>
+          <a:ext cx="666750" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="sysDash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="直線コネクタ 23"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5495925" y="3933825"/>
+          <a:ext cx="695325" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="sysDash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="直線コネクタ 25"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2714625" y="4105275"/>
+          <a:ext cx="723900" cy="542925"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="直線コネクタ 27"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4457700" y="4124325"/>
+          <a:ext cx="9525" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="直線コネクタ 29"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5486400" y="4124325"/>
+          <a:ext cx="1352550" cy="476250"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1001,7 +1788,7 @@
   <dimension ref="A2:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD25"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1050,9 +1837,9 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="1"/>
+        <v>63</v>
+      </c>
+      <c r="C7" s="21"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9" s="9" t="s">
@@ -1061,7 +1848,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.15">
@@ -1094,13 +1881,13 @@
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F12" s="14" t="s">
         <v>30</v>
@@ -1116,7 +1903,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>10</v>
@@ -1132,12 +1919,12 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A16" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A17" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.15">
@@ -1193,13 +1980,13 @@
         <v>17</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G20" s="10"/>
       <c r="H20" s="11"/>
@@ -1215,7 +2002,7 @@
         <v>18</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>27</v>
@@ -1236,13 +2023,13 @@
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F22" s="1">
         <v>10</v>
@@ -1305,7 +2092,7 @@
         <v>21</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>27</v>
@@ -1343,7 +2130,7 @@
   <dimension ref="A2:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:C23"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1371,7 +2158,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
@@ -1379,7 +2166,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
@@ -1392,7 +2179,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -1403,7 +2190,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.15">
@@ -1437,13 +2224,13 @@
         <v>17</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="11"/>
@@ -1458,7 +2245,7 @@
         <v>18</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>10</v>
@@ -1478,19 +2265,19 @@
         <v>3</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E14" s="1">
         <v>10</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
@@ -1546,7 +2333,7 @@
         <v>21</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>10</v>
@@ -1562,12 +2349,12 @@
     <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1592,7 +2379,7 @@
   <dimension ref="A2:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1612,7 +2399,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
@@ -1620,7 +2407,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
@@ -1628,7 +2415,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
@@ -1641,29 +2428,29 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" s="1"/>
+        <v>65</v>
+      </c>
+      <c r="C7" s="21"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9" s="9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10" s="9" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13" s="9" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
@@ -1697,14 +2484,14 @@
         <v>1</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="7"/>
       <c r="G15" s="17" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="H15" s="17"/>
       <c r="I15" s="17"/>
@@ -1719,10 +2506,10 @@
         <v>12</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F16" s="1">
         <v>3</v>
@@ -1740,13 +2527,13 @@
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F17" s="1">
         <v>10</v>
@@ -1770,4 +2557,222 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:P28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.15">
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.15">
+      <c r="B3" s="21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.15">
+      <c r="B4" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="23"/>
+      <c r="D4" s="24"/>
+      <c r="F4" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.15">
+      <c r="B5" s="25"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="27"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="27"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.15">
+      <c r="J6" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="K6" s="23"/>
+      <c r="L6" s="24"/>
+      <c r="N6" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="O6" s="23"/>
+      <c r="P6" s="24"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.15">
+      <c r="J7" s="25"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="27"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="27"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.15">
+      <c r="D8" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" s="23"/>
+      <c r="F8" s="24"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.15">
+      <c r="D9" s="25"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="27"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.15">
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.15">
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="28"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.15">
+      <c r="B12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.15">
+      <c r="B13" s="21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.15">
+      <c r="B14" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="23"/>
+      <c r="D14" s="24"/>
+      <c r="F14" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" s="23"/>
+      <c r="H14" s="24"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.15">
+      <c r="B15" s="25"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="27"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="27"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="D17" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="23"/>
+      <c r="F17" s="24"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="D18" s="25"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="27"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B22" s="21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B23" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="23"/>
+      <c r="D23" s="24"/>
+      <c r="F23" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="G23" s="23"/>
+      <c r="H23" s="24"/>
+      <c r="J23" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="K23" s="23"/>
+      <c r="L23" s="24"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B24" s="25"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="27"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="27"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="27"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="F27" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="G27" s="23"/>
+      <c r="H27" s="24"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="F28" s="25"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="27"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="D17:F18"/>
+    <mergeCell ref="D8:F9"/>
+    <mergeCell ref="B23:D24"/>
+    <mergeCell ref="F23:H24"/>
+    <mergeCell ref="J23:L24"/>
+    <mergeCell ref="F27:H28"/>
+    <mergeCell ref="N6:P7"/>
+    <mergeCell ref="B4:D5"/>
+    <mergeCell ref="F4:H5"/>
+    <mergeCell ref="J6:L7"/>
+    <mergeCell ref="B14:D15"/>
+    <mergeCell ref="F14:H15"/>
+  </mergeCells>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add src, mod APIdoc
</commit_message>
<xml_diff>
--- a/API定義書.xlsx
+++ b/API定義書.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="14805" windowHeight="7995" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="14805" windowHeight="7980" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="購入履歴一覧表示API" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="86">
   <si>
     <t>API和名</t>
     <rPh sb="3" eb="5">
@@ -363,16 +363,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>返却オブジェクト英名：List&lt;PaymentInfo&gt;</t>
-    <rPh sb="0" eb="2">
-      <t>ヘンキャク</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>エイメイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>呼出パラメータオブジェクト英名：PaymentInfo</t>
     <rPh sb="0" eb="2">
       <t>ヨビダシ</t>
@@ -431,16 +421,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>返却オブジェクト英名：List&lt;Item&gt;</t>
-    <rPh sb="0" eb="2">
-      <t>ヘンキャク</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>エイメイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>品目一覧</t>
     <rPh sb="0" eb="2">
       <t>ヒンモク</t>
@@ -513,18 +493,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>PaymentListRestController</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>PaymentListRepositoryService</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>PaymentListService</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>支払詳細API</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -533,14 +501,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>PaymentDetailRestController</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>PaymentDetailService</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>品目一覧取得API</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -549,18 +509,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>GetItemListRestController</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>GetItemListService</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>GetItemListRepositoryService</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Item</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -574,6 +522,91 @@
   </si>
   <si>
     <t>QueryInfo</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>POST: api/getItemList/</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>返却オブジェクト英名：Itemlist</t>
+    <rPh sb="0" eb="2">
+      <t>ヘンキャク</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>エイメイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>オブジェクト英名</t>
+    <rPh sb="6" eb="8">
+      <t>エイメイ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>メイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>itemlist</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>返却オブジェクト英名：paymentInfoList</t>
+    <rPh sb="0" eb="2">
+      <t>ヘンキャク</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>エイメイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>paymentInfoList</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ItemListRepository
+- selectAll</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>GetItemListService
+- selectAll</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>GetItemListRestController
+- getItemList</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PaymentListRestController
+- getPaymentList</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PaymentListRepository
+- selectAll
+- insertPayment</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PaymentDetailRestController
+- insertPayment</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PaymentDetailService
+- insertPayment
++ conversionToJson</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PaymentListService
+- selectAll
++ conversionToJson</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -641,30 +674,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -766,58 +775,92 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -829,14 +872,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1041,13 +1107,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>409576</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1058,8 +1124,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="5210175" y="1257300"/>
-          <a:ext cx="1095375" cy="971550"/>
+          <a:off x="5210176" y="1438275"/>
+          <a:ext cx="904874" cy="790575"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1785,22 +1851,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J26"/>
+  <dimension ref="A2:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="13.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5" customWidth="1"/>
-    <col min="5" max="5" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.25" customWidth="1"/>
-    <col min="7" max="7" width="17.25" customWidth="1"/>
-    <col min="8" max="8" width="11" customWidth="1"/>
-    <col min="10" max="10" width="15.125" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="5" max="5" width="17.5" customWidth="1"/>
+    <col min="6" max="6" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.25" customWidth="1"/>
+    <col min="8" max="8" width="17.25" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="11" max="11" width="15.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
@@ -1810,6 +1877,7 @@
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="C2" s="11"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
@@ -1818,6 +1886,7 @@
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C3" s="11"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
@@ -1831,23 +1900,25 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" s="21"/>
+        <v>61</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="7" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1867,11 +1938,11 @@
       <c r="E11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="23"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
@@ -1889,11 +1960,11 @@
       <c r="E12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="16"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
@@ -1918,16 +1989,16 @@
       <c r="H13" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A17" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A17" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
@@ -1935,189 +2006,200 @@
         <v>24</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="F18" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="G18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="13" t="s">
+      <c r="H18" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A19" s="1">
         <v>1</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="17" t="s">
+      <c r="C19" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A20" s="1">
         <v>2</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="1" t="s">
+      <c r="B20" s="31"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G20" s="10"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="12"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="H20" s="13"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="15"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A21" s="1">
         <v>3</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="1" t="s">
+      <c r="B21" s="31"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="E21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F21" s="1">
+      <c r="G21" s="1">
         <v>3</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="H21" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="12"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="15"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A22" s="1">
         <v>4</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="1" t="s">
+      <c r="B22" s="31"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F22" s="1">
+      <c r="G22" s="1">
         <v>10</v>
       </c>
-      <c r="G22" s="10"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="12"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="H22" s="13"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="15"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A23" s="1">
         <v>5</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="1" t="s">
+      <c r="B23" s="31"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F23" s="1">
+      <c r="G23" s="1">
         <v>7</v>
       </c>
-      <c r="G23" s="10"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="12"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="H23" s="13"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="15"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A24" s="1">
         <v>6</v>
       </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="1" t="s">
+      <c r="B24" s="31"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F24" s="1">
+      <c r="G24" s="1">
         <v>3</v>
       </c>
-      <c r="G24" s="10"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="12"/>
-    </row>
-    <row r="25" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H24" s="13"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="15"/>
+    </row>
+    <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1">
         <v>7</v>
       </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="1" t="s">
+      <c r="B25" s="33"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F25" s="1">
+      <c r="G25" s="1">
         <v>10</v>
       </c>
-      <c r="G25" s="10"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="12"/>
-    </row>
-    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="15"/>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="G25:J25"/>
+  <mergeCells count="9">
     <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="G19:J19"/>
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="G24:J24"/>
-    <mergeCell ref="G22:J22"/>
+    <mergeCell ref="H25:K25"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="H19:K19"/>
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="H21:K21"/>
+    <mergeCell ref="H23:K23"/>
+    <mergeCell ref="H24:K24"/>
+    <mergeCell ref="H22:K22"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2158,39 +2240,39 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="16"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="19"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A10" s="9" t="s">
-        <v>45</v>
+      <c r="A10" s="7" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.15">
@@ -2209,12 +2291,12 @@
       <c r="E11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="20"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="23"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
@@ -2232,10 +2314,10 @@
       <c r="E12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="12"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="15"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
@@ -2253,22 +2335,22 @@
       <c r="E13" s="1">
         <v>3</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="12"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="15"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
         <v>3</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>39</v>
@@ -2276,12 +2358,12 @@
       <c r="E14" s="1">
         <v>10</v>
       </c>
-      <c r="F14" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="12"/>
+      <c r="F14" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="15"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
@@ -2299,10 +2381,10 @@
       <c r="E15" s="1">
         <v>7</v>
       </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="12"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="15"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="1">
@@ -2320,10 +2402,10 @@
       <c r="E16" s="1">
         <v>3</v>
       </c>
-      <c r="F16" s="10"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="12"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="15"/>
     </row>
     <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1">
@@ -2341,14 +2423,14 @@
       <c r="E17" s="1">
         <v>10</v>
       </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="12"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="15"/>
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="19" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="7" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2376,84 +2458,89 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J17"/>
+  <dimension ref="A2:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="13.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5" customWidth="1"/>
-    <col min="5" max="5" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.25" customWidth="1"/>
-    <col min="7" max="7" width="17.25" customWidth="1"/>
-    <col min="8" max="8" width="11" customWidth="1"/>
-    <col min="10" max="10" width="15.125" customWidth="1"/>
+    <col min="3" max="3" width="14.125" customWidth="1"/>
+    <col min="5" max="5" width="17.5" customWidth="1"/>
+    <col min="6" max="6" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.25" customWidth="1"/>
+    <col min="8" max="8" width="17.25" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="11" max="11" width="15.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+        <v>48</v>
+      </c>
+      <c r="C2" s="11"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+        <v>67</v>
+      </c>
+      <c r="C3" s="11"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="16"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B5" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="19"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="21"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A9" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A9" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A10" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A10" s="9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A12" s="9" t="s">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A12" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A13" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A13" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
         <v>6</v>
       </c>
@@ -2461,97 +2548,105 @@
         <v>24</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="G14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="H14" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
         <v>1</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B15" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A16" s="1">
         <v>2</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="1" t="s">
+      <c r="B16" s="31"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="E16" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F16" s="1">
+        <v>60</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="1">
         <v>3</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="H16" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="12"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="15"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A17" s="1">
         <v>3</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="B17" s="33"/>
+      <c r="C17" s="34"/>
       <c r="D17" s="1" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F17" s="1">
+        <v>54</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" s="1">
         <v>10</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="H17" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="12"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="H17:K17"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2563,213 +2658,213 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K14:K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.15">
+      <c r="B3" s="11" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B3" s="21" t="s">
-        <v>63</v>
-      </c>
-    </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B4" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="24"/>
-      <c r="F4" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="G4" s="23"/>
-      <c r="H4" s="24"/>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B5" s="25"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="27"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="27"/>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="J6" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="K6" s="23"/>
-      <c r="L6" s="24"/>
-      <c r="N6" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="O6" s="23"/>
-      <c r="P6" s="24"/>
+      <c r="B4" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="25"/>
+      <c r="D4" s="26"/>
+      <c r="F4" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" s="25"/>
+      <c r="H4" s="26"/>
+    </row>
+    <row r="5" spans="2:16" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B5" s="27"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="29"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="29"/>
+    </row>
+    <row r="6" spans="2:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J6" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="K6" s="36"/>
+      <c r="L6" s="38"/>
+      <c r="N6" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="O6" s="25"/>
+      <c r="P6" s="26"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="J7" s="25"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="27"/>
-      <c r="N7" s="25"/>
-      <c r="O7" s="26"/>
-      <c r="P7" s="27"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="40"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="29"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="D8" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="E8" s="23"/>
-      <c r="F8" s="24"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
-      <c r="N8" s="28"/>
-      <c r="O8" s="28"/>
-      <c r="P8" s="28"/>
+      <c r="D8" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="25"/>
+      <c r="F8" s="26"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="43"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="D9" s="25"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="27"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="28"/>
-      <c r="P9" s="28"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="29"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="28"/>
-      <c r="N10" s="28"/>
-      <c r="O10" s="28"/>
-      <c r="P10" s="28"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="28"/>
-      <c r="N11" s="28"/>
-      <c r="O11" s="28"/>
-      <c r="P11" s="28"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B13" s="21" t="s">
-        <v>64</v>
+      <c r="B13" s="11" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B14" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="24"/>
-      <c r="F14" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="G14" s="23"/>
-      <c r="H14" s="24"/>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B15" s="25"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="27"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="27"/>
+      <c r="B14" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="25"/>
+      <c r="D14" s="26"/>
+      <c r="F14" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" s="25"/>
+      <c r="H14" s="26"/>
+    </row>
+    <row r="15" spans="2:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B15" s="27"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="29"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="29"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="D17" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="E17" s="23"/>
-      <c r="F17" s="24"/>
+      <c r="D17" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" s="25"/>
+      <c r="F17" s="26"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="D18" s="25"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="29"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B21" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B22" s="21" t="s">
-        <v>65</v>
+      <c r="B22" s="11" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B23" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="C23" s="23"/>
-      <c r="D23" s="24"/>
-      <c r="F23" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="G23" s="23"/>
-      <c r="H23" s="24"/>
-      <c r="J23" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="K23" s="23"/>
-      <c r="L23" s="24"/>
+      <c r="B23" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" s="25"/>
+      <c r="D23" s="26"/>
+      <c r="F23" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="G23" s="25"/>
+      <c r="H23" s="26"/>
+      <c r="J23" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="K23" s="25"/>
+      <c r="L23" s="26"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B24" s="25"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="27"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="27"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="27"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="29"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="29"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="29"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="F27" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="G27" s="23"/>
-      <c r="H27" s="24"/>
+      <c r="F27" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="G27" s="25"/>
+      <c r="H27" s="26"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="F28" s="25"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="F27:H28"/>
+    <mergeCell ref="N6:P7"/>
+    <mergeCell ref="B4:D5"/>
+    <mergeCell ref="F4:H5"/>
+    <mergeCell ref="B14:D15"/>
+    <mergeCell ref="F14:H15"/>
+    <mergeCell ref="J6:L8"/>
     <mergeCell ref="D17:F18"/>
     <mergeCell ref="D8:F9"/>
     <mergeCell ref="B23:D24"/>
     <mergeCell ref="F23:H24"/>
     <mergeCell ref="J23:L24"/>
-    <mergeCell ref="F27:H28"/>
-    <mergeCell ref="N6:P7"/>
-    <mergeCell ref="B4:D5"/>
-    <mergeCell ref="F4:H5"/>
-    <mergeCell ref="J6:L7"/>
-    <mergeCell ref="B14:D15"/>
-    <mergeCell ref="F14:H15"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>